<commit_message>
se escribio jersson romero
</commit_message>
<xml_diff>
--- a/Nuevo Hoja de cálculo de Microsoft Excel.xlsx
+++ b/Nuevo Hoja de cálculo de Microsoft Excel.xlsx
@@ -19,9 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>jerardo romero</t>
+  </si>
+  <si>
+    <t>jersson romero</t>
   </si>
 </sst>
 </file>
@@ -339,10 +342,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3"/>
+  <dimension ref="C3:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -352,6 +355,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "se escribio jersson romero"
This reverts commit 2788f38b029711133671ff8a60c82509ba7abeba.
</commit_message>
<xml_diff>
--- a/Nuevo Hoja de cálculo de Microsoft Excel.xlsx
+++ b/Nuevo Hoja de cálculo de Microsoft Excel.xlsx
@@ -19,12 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>jerardo romero</t>
-  </si>
-  <si>
-    <t>jersson romero</t>
   </si>
 </sst>
 </file>
@@ -342,10 +339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:C4"/>
+  <dimension ref="C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -355,11 +352,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Revert "se escribio jersson romero""
This reverts commit d18490a5a4eda6cbaaf8699a5dbdc11f96a8080f.
</commit_message>
<xml_diff>
--- a/Nuevo Hoja de cálculo de Microsoft Excel.xlsx
+++ b/Nuevo Hoja de cálculo de Microsoft Excel.xlsx
@@ -19,9 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>jerardo romero</t>
+  </si>
+  <si>
+    <t>jersson romero</t>
   </si>
 </sst>
 </file>
@@ -339,10 +342,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3"/>
+  <dimension ref="C3:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -352,6 +355,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>